<commit_message>
Actualizo archivos de brechas de ingresos por región
</commit_message>
<xml_diff>
--- a/Datos/BRECHAS_ING/Brechas_Ingresos_Region_1.xlsx
+++ b/Datos/BRECHAS_ING/Brechas_Ingresos_Region_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\sfarias\Documents\Curso Python\.vscode\dashboard-indicadores\Datos\BRECHAS_ING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BDE7E7-12D4-4047-8E28-9A0DF6D3051E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C561710-AA76-460A-940D-B7A9730EAB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,10 +82,10 @@
     <t>Region de Tarapacá</t>
   </si>
   <si>
-    <t>Masculino</t>
-  </si>
-  <si>
-    <t>Femenino</t>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>Mujer</t>
   </si>
 </sst>
 </file>

</xml_diff>